<commit_message>
redoing interRR- error with excel sheet!
</commit_message>
<xml_diff>
--- a/PAPER_1/inter_ICC_all.xlsx
+++ b/PAPER_1/inter_ICC_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colostate-my.sharepoint.com/personal/khobbs01_colostate_edu/Documents/Desktop/Dissertation/headscan_dissertation/PAPER_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_F25DC773A252ABDACC1048E4D1DD70DA5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D418548E-061F-49C5-BDDB-2238C395D0CC}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_F25DC773A252ABDACC1048E4D1DD70DA5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DC68902-9EE3-4390-B1AB-FE1366323B5D}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,208 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -475,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56:E82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +710,13 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.94399999999999995</v>
+        <v>0.874</v>
       </c>
       <c r="C2">
-        <v>0.83499999999999996</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="D2">
-        <v>0.98499999999999999</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -529,13 +730,13 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.67500000000000004</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="C3">
-        <v>-1.2E-2</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="D3">
-        <v>0.91400000000000003</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -549,13 +750,13 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.745</v>
+        <v>-0.20100000000000001</v>
       </c>
       <c r="C4">
-        <v>0.27500000000000002</v>
+        <v>-0.71799999999999997</v>
       </c>
       <c r="D4">
-        <v>0.93</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -569,13 +770,13 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0.85899999999999999</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="C5">
-        <v>0.54600000000000004</v>
+        <v>-0.158</v>
       </c>
       <c r="D5">
-        <v>0.96299999999999997</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -589,13 +790,13 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>0.96799999999999997</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="C6">
-        <v>0.90700000000000003</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="D6">
-        <v>0.99199999999999999</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -609,13 +810,13 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>0.41799999999999998</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="C7">
-        <v>-0.59599999999999997</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D7">
-        <v>0.85</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -629,13 +830,13 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.89100000000000001</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="C8">
-        <v>0.69299999999999995</v>
+        <v>0.253</v>
       </c>
       <c r="D8">
-        <v>0.97</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -649,13 +850,13 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>0.82399999999999995</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="C9">
-        <v>0.48599999999999999</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="D9">
-        <v>0.95199999999999996</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -669,13 +870,13 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>0.71499999999999997</v>
+        <v>0.75</v>
       </c>
       <c r="C10">
-        <v>0.15</v>
+        <v>0.37</v>
       </c>
       <c r="D10">
-        <v>0.92400000000000004</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -689,13 +890,13 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>0.90700000000000003</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="C11">
-        <v>0.73</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="D11">
-        <v>0.97499999999999998</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -709,13 +910,13 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>0.93799999999999994</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C12">
-        <v>0.81699999999999995</v>
+        <v>0.435</v>
       </c>
       <c r="D12">
-        <v>0.98299999999999998</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -729,13 +930,13 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>0.89900000000000002</v>
+        <v>0.86</v>
       </c>
       <c r="C13">
-        <v>0.71599999999999997</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="D13">
-        <v>0.97199999999999998</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -749,13 +950,13 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>0.90600000000000003</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="C14">
-        <v>0.73299999999999998</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="D14">
-        <v>0.97499999999999998</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -769,13 +970,13 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>0.69799999999999995</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="C15">
-        <v>0.155</v>
+        <v>-0.24399999999999999</v>
       </c>
       <c r="D15">
-        <v>0.91600000000000004</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -789,13 +990,13 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <v>0.95799999999999996</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="C16">
-        <v>0.872</v>
+        <v>0.434</v>
       </c>
       <c r="D16">
-        <v>0.98899999999999999</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -809,13 +1010,13 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>0.93300000000000005</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="C17">
-        <v>0.79800000000000004</v>
+        <v>0.39</v>
       </c>
       <c r="D17">
-        <v>0.98299999999999998</v>
+        <v>0.97</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -829,13 +1030,13 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>0.66100000000000003</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="C18">
-        <v>4.1000000000000002E-2</v>
+        <v>-2.5880000000000001</v>
       </c>
       <c r="D18">
-        <v>0.91400000000000003</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -849,13 +1050,13 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>0.60799999999999998</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="C19">
-        <v>-8.5999999999999993E-2</v>
+        <v>-1.895</v>
       </c>
       <c r="D19">
-        <v>0.89900000000000002</v>
+        <v>0.872</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -869,13 +1070,13 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>0.94699999999999995</v>
+        <v>0.86</v>
       </c>
       <c r="C20">
-        <v>0.83799999999999997</v>
+        <v>0.443</v>
       </c>
       <c r="D20">
-        <v>0.98699999999999999</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -889,13 +1090,13 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>0.92600000000000005</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="C21">
-        <v>0.77800000000000002</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="D21">
-        <v>0.98199999999999998</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -909,13 +1110,13 @@
         <v>30</v>
       </c>
       <c r="B22">
-        <v>0.91800000000000004</v>
+        <v>0.753</v>
       </c>
       <c r="C22">
-        <v>0.66500000000000004</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="D22">
-        <v>0.98099999999999998</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -929,13 +1130,13 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>0.86899999999999999</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="C23">
-        <v>0.54700000000000004</v>
+        <v>0.317</v>
       </c>
       <c r="D23">
-        <v>0.97199999999999998</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -949,13 +1150,13 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>0.98699999999999999</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="C24">
-        <v>0.96</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="D24">
-        <v>0.997</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -969,13 +1170,13 @@
         <v>33</v>
       </c>
       <c r="B25">
-        <v>0.71099999999999997</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="C25">
-        <v>0.1</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="D25">
-        <v>0.93600000000000005</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -989,13 +1190,13 @@
         <v>34</v>
       </c>
       <c r="B26">
-        <v>0.995</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="C26">
-        <v>0.98299999999999998</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="D26">
-        <v>0.999</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1009,13 +1210,13 @@
         <v>35</v>
       </c>
       <c r="B27">
-        <v>0.98799999999999999</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="C27">
-        <v>0.96299999999999997</v>
+        <v>0.9</v>
       </c>
       <c r="D27">
-        <v>0.997</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1029,13 +1230,13 @@
         <v>36</v>
       </c>
       <c r="B28">
-        <v>0.97799999999999998</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="C28">
-        <v>0.93500000000000005</v>
+        <v>0.12</v>
       </c>
       <c r="D28">
-        <v>0.995</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>

</xml_diff>